<commit_message>
before apllying last changes from pablo last two commits
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -1,63 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codebase\UISpiceJet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AADC1D-26AB-4269-B6B7-AA07E7A69FA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB95A458-48E6-40DF-A760-658141830EE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23325" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACC7127D-CA10-4415-AB1E-B8CD0C7426B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>FROM</t>
-  </si>
-  <si>
-    <t>TO</t>
-  </si>
-  <si>
-    <t>DEPARTURE_DATE</t>
-  </si>
-  <si>
-    <t>ARRIVAL_DATE</t>
-  </si>
-  <si>
-    <t>ADULTS</t>
-  </si>
-  <si>
-    <t>CHILDREN</t>
-  </si>
-  <si>
-    <t>Flight_From_Mexico_to_Canada</t>
-  </si>
-  <si>
-    <t>MEXICO</t>
-  </si>
-  <si>
-    <t>CANADA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>October 20 2020</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>adults</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>departure</t>
+  </si>
+  <si>
+    <t>arrival</t>
+  </si>
+  <si>
+    <t>Test_1</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>infant</t>
+  </si>
+  <si>
+    <t>One way</t>
+  </si>
+  <si>
+    <t>MONTERREY</t>
+  </si>
+  <si>
+    <t>CHIHUAHUA</t>
+  </si>
+  <si>
+    <t>Test_2</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
 </sst>
 </file>
@@ -73,10 +97,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,14 +123,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,7 +159,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -153,7 +171,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -200,6 +218,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -235,6 +270,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -386,72 +438,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACA775C-E285-4133-A09C-4B3E0732D713}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>